<commit_message>
- this file was modified second time
</commit_message>
<xml_diff>
--- a/Excel_version_control demo.xlsx
+++ b/Excel_version_control demo.xlsx
@@ -16,12 +16,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t># The purpose of this excel sheet is to check whether github incorporate manual changes.</t>
+    <t>#2. this cell was added in the second version</t>
   </si>
   <si>
-    <t>#1. this is the first version of file</t>
+    <t>#3. this earlier cell was modified to this text</t>
+  </si>
+  <si>
+    <t>Added</t>
+  </si>
+  <si>
+    <t>Modified</t>
+  </si>
+  <si>
+    <t>deleted</t>
   </si>
 </sst>
 </file>
@@ -360,22 +369,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
+      <c r="B5" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>